<commit_message>
Update dictionary and other changes
</commit_message>
<xml_diff>
--- a/raw/codal_raw/part_2/شسپا/نفت سپاهان-55/Balance Sheet.xlsx
+++ b/raw/codal_raw/part_2/شسپا/نفت سپاهان-55/Balance Sheet.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_project\FirmFSCleansing\raw\codal_raw\part_2\شسپا\نفت سپاهان-55\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8789E01F-67B9-403E-9B7D-D435BE2A2459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="19890" yWindow="4335" windowWidth="17145" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="135">
   <si>
     <t>nemad</t>
   </si>
@@ -419,13 +425,16 @@
   </si>
   <si>
     <t>Balance Sheet</t>
+  </si>
+  <si>
+    <t>شسپا</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,6 +497,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -534,7 +551,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -566,9 +583,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,6 +635,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -775,14 +828,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -832,12 +890,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M2" t="s">
         <v>129</v>
@@ -855,12 +913,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M3" t="s">
         <v>129</v>
@@ -878,12 +936,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M4" t="s">
         <v>129</v>
@@ -901,12 +959,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="L5" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M5" t="s">
         <v>129</v>
@@ -924,12 +982,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M6" t="s">
         <v>129</v>
@@ -947,12 +1005,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="L7" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M7" t="s">
         <v>129</v>
@@ -970,12 +1028,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="L8" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M8" t="s">
         <v>129</v>
@@ -993,12 +1051,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="L9" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M9" t="s">
         <v>129</v>
@@ -1016,12 +1074,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="L10" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M10" t="s">
         <v>129</v>
@@ -1039,12 +1097,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="L11" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M11" t="s">
         <v>129</v>
@@ -1062,12 +1120,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M12" t="s">
         <v>129</v>
@@ -1085,12 +1143,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="L13" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M13" t="s">
         <v>129</v>
@@ -1108,12 +1166,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="L14" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M14" t="s">
         <v>129</v>
@@ -1131,7 +1189,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1160,7 +1218,7 @@
         <v>56</v>
       </c>
       <c r="L15" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M15" t="s">
         <v>129</v>
@@ -1178,12 +1236,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="L16" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M16" t="s">
         <v>129</v>
@@ -1201,7 +1259,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1212,7 +1270,7 @@
         <v>71</v>
       </c>
       <c r="L17" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M17" t="s">
         <v>129</v>
@@ -1230,7 +1288,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1250,7 +1308,7 @@
         <v>72</v>
       </c>
       <c r="L18" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M18" t="s">
         <v>129</v>
@@ -1268,7 +1326,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1297,7 +1355,7 @@
         <v>122</v>
       </c>
       <c r="L19" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M19" t="s">
         <v>129</v>
@@ -1315,7 +1373,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1344,7 +1402,7 @@
         <v>60</v>
       </c>
       <c r="L20" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M20" t="s">
         <v>129</v>
@@ -1362,7 +1420,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1391,7 +1449,7 @@
         <v>123</v>
       </c>
       <c r="L21" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M21" t="s">
         <v>129</v>
@@ -1409,7 +1467,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1438,7 +1496,7 @@
         <v>124</v>
       </c>
       <c r="L22" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M22" t="s">
         <v>129</v>
@@ -1456,7 +1514,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1485,7 +1543,7 @@
         <v>125</v>
       </c>
       <c r="L23" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M23" t="s">
         <v>129</v>
@@ -1503,7 +1561,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1532,7 +1590,7 @@
         <v>60</v>
       </c>
       <c r="L24" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M24" t="s">
         <v>129</v>
@@ -1550,7 +1608,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1579,7 +1637,7 @@
         <v>61</v>
       </c>
       <c r="L25" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M25" t="s">
         <v>129</v>
@@ -1597,7 +1655,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1626,7 +1684,7 @@
         <v>60</v>
       </c>
       <c r="L26" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M26" t="s">
         <v>129</v>
@@ -1644,7 +1702,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1673,7 +1731,7 @@
         <v>126</v>
       </c>
       <c r="L27" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M27" t="s">
         <v>129</v>
@@ -1691,7 +1749,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1702,7 +1760,7 @@
         <v>82</v>
       </c>
       <c r="L28" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M28" t="s">
         <v>129</v>
@@ -1720,7 +1778,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1749,7 +1807,7 @@
         <v>60</v>
       </c>
       <c r="L29" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M29" t="s">
         <v>129</v>
@@ -1767,7 +1825,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1796,7 +1854,7 @@
         <v>60</v>
       </c>
       <c r="L30" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M30" t="s">
         <v>129</v>
@@ -1814,7 +1872,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1843,7 +1901,7 @@
         <v>127</v>
       </c>
       <c r="L31" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M31" t="s">
         <v>129</v>
@@ -1861,7 +1919,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1890,7 +1948,7 @@
         <v>127</v>
       </c>
       <c r="L32" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M32" t="s">
         <v>129</v>
@@ -1908,7 +1966,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1937,7 +1995,7 @@
         <v>126</v>
       </c>
       <c r="L33" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M33" t="s">
         <v>129</v>
@@ -1955,7 +2013,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1975,7 +2033,7 @@
         <v>88</v>
       </c>
       <c r="L34" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M34" t="s">
         <v>129</v>
@@ -1993,7 +2051,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2010,7 +2068,7 @@
         <v>30</v>
       </c>
       <c r="L35" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M35" t="s">
         <v>129</v>
@@ -2028,7 +2086,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2045,7 +2103,7 @@
         <v>60</v>
       </c>
       <c r="L36" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M36" t="s">
         <v>129</v>
@@ -2063,7 +2121,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2080,7 +2138,7 @@
         <v>60</v>
       </c>
       <c r="L37" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M37" t="s">
         <v>129</v>
@@ -2098,7 +2156,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2115,7 +2173,7 @@
         <v>30</v>
       </c>
       <c r="L38" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M38" t="s">
         <v>129</v>
@@ -2133,7 +2191,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2150,7 +2208,7 @@
         <v>60</v>
       </c>
       <c r="L39" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M39" t="s">
         <v>129</v>
@@ -2168,7 +2226,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2185,7 +2243,7 @@
         <v>60</v>
       </c>
       <c r="L40" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M40" t="s">
         <v>129</v>
@@ -2203,7 +2261,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2220,7 +2278,7 @@
         <v>60</v>
       </c>
       <c r="L41" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M41" t="s">
         <v>129</v>
@@ -2238,7 +2296,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2255,7 +2313,7 @@
         <v>60</v>
       </c>
       <c r="L42" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M42" t="s">
         <v>129</v>
@@ -2273,7 +2331,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2290,7 +2348,7 @@
         <v>128</v>
       </c>
       <c r="L43" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M43" t="s">
         <v>129</v>
@@ -2308,7 +2366,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2325,7 +2383,7 @@
         <v>64</v>
       </c>
       <c r="L44" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M44" t="s">
         <v>129</v>
@@ -2343,7 +2401,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2372,7 +2430,7 @@
         <v>70</v>
       </c>
       <c r="L45" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M45" t="s">
         <v>129</v>

</xml_diff>